<commit_message>
Modifique detalles en municipios
</commit_message>
<xml_diff>
--- a/insezacweb/assets/files/beneficiarios.xlsx
+++ b/insezacweb/assets/files/beneficiarios.xlsx
@@ -372,7 +372,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,14 +405,6 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -483,9 +475,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -507,11 +499,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -796,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1:AM1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +980,7 @@
       <c r="J2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>97</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -1058,7 +1049,7 @@
       <c r="AG2" s="4">
         <v>2</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AH2" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI2" s="4"/>
@@ -1098,7 +1089,7 @@
       <c r="J3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>98</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -1167,7 +1158,7 @@
       <c r="AG3" s="4">
         <v>2</v>
       </c>
-      <c r="AH3" s="9" t="s">
+      <c r="AH3" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI3" s="4"/>
@@ -1207,7 +1198,7 @@
       <c r="J4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>99</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -1276,7 +1267,7 @@
       <c r="AG4" s="4">
         <v>2</v>
       </c>
-      <c r="AH4" s="9" t="s">
+      <c r="AH4" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI4" s="4"/>
@@ -1316,7 +1307,7 @@
       <c r="J5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>100</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -1385,7 +1376,7 @@
       <c r="AG5" s="4">
         <v>2</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AH5" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI5" s="4"/>
@@ -1425,7 +1416,7 @@
       <c r="J6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -1494,7 +1485,7 @@
       <c r="AG6" s="4">
         <v>2</v>
       </c>
-      <c r="AH6" s="9" t="s">
+      <c r="AH6" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI6" s="4"/>
@@ -1534,7 +1525,7 @@
       <c r="J7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>102</v>
       </c>
       <c r="L7" s="4" t="s">
@@ -1603,7 +1594,7 @@
       <c r="AG7" s="4">
         <v>2</v>
       </c>
-      <c r="AH7" s="9" t="s">
+      <c r="AH7" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI7" s="4"/>
@@ -1643,7 +1634,7 @@
       <c r="J8" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>103</v>
       </c>
       <c r="L8" s="4" t="s">
@@ -1712,7 +1703,7 @@
       <c r="AG8" s="4">
         <v>2</v>
       </c>
-      <c r="AH8" s="9" t="s">
+      <c r="AH8" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI8" s="4"/>
@@ -1752,7 +1743,7 @@
       <c r="J9" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>104</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -1821,7 +1812,7 @@
       <c r="AG9" s="4">
         <v>2</v>
       </c>
-      <c r="AH9" s="9" t="s">
+      <c r="AH9" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI9" s="4"/>
@@ -1861,7 +1852,7 @@
       <c r="J10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>105</v>
       </c>
       <c r="L10" s="4" t="s">
@@ -1930,7 +1921,7 @@
       <c r="AG10" s="4">
         <v>2</v>
       </c>
-      <c r="AH10" s="9" t="s">
+      <c r="AH10" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI10" s="4"/>
@@ -1970,7 +1961,7 @@
       <c r="J11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>106</v>
       </c>
       <c r="L11" s="4" t="s">
@@ -2039,7 +2030,7 @@
       <c r="AG11" s="4">
         <v>2</v>
       </c>
-      <c r="AH11" s="9" t="s">
+      <c r="AH11" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AI11" s="4"/>
@@ -2049,7 +2040,161 @@
       <c r="AM11" s="4"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="L12" s="7"/>
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>A12+1</f>
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <f>B12+1</f>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:AM12" si="0">C12+1</f>
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>